<commit_message>
Added Support for SENSe:VOLTage Commands
</commit_message>
<xml_diff>
--- a/34461A to 2600.xlsx
+++ b/34461A to 2600.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ralliant-my.sharepoint.com/personal/oliver_bindewald_tektronix_com/Documents/Documents/DMM6500 Emulation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ralliant-my.sharepoint.com/personal/oliver_bindewald_tektronix_com/Documents/Documents/DMM6500 Emulation/34461A-Emulator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="454" documentId="11_F25DC773A252ABDACC1048A921D94B805ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70425F5F-3DA7-4F80-B5FD-3178A9692CB6}"/>
+  <xr:revisionPtr revIDLastSave="574" documentId="11_F25DC773A252ABDACC1048A921D94B805ADE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06D4DFD7-8694-43C8-B147-37FB640B5CAB}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7935" windowWidth="16440" windowHeight="29040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="488">
   <si>
     <t>34461A SCPI</t>
   </si>
@@ -1439,200 +1439,28 @@
     <t>STATus:QUEStionable[:EVENt]?</t>
   </si>
   <si>
-    <t>print(dmm.measure.func, dmm.measure.range, dmm.measure.displaydigits)
-print(dmm.digitize.func, dmm.digitize.range dmm.measure.displaydigits)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dmm.measure.func = dmm.FUNC_CAPACITANCE
-dmm.measure.range = 
-dmm.measure.displaydigits = </t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_CONTINUITY</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_DC|AC_CURRENT
-dmm.measure.range = 
-dmm.measure.displaydigits =</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_DIODE</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_ACV_FREQUENCY|PERIOD
-dmm.measure.range =
-dmm.measure.displaydigits =</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC _RESISTANCE|4W_RESISTANCE
-dmm.measure.range =
-dmm.measure.displaydigits =</t>
-  </si>
-  <si>
     <t>Check some of these parameters</t>
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>dmm.measure.displaydigits =</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_DC|AC_VOLTAGE
-dmm.measure.range = 
-dmm.measure.displaydigits =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dmm.measure.func = dmm.FUNC_DCV_AUTO
-dmm.measure.range =
-dmm.measure.displaydigits = </t>
-  </si>
-  <si>
-    <t>DMM6500 TSP</t>
   </si>
   <si>
     <t>Resolution Ignored and set to 4.5 digits
 Figure out how reading buffers should be handled</t>
   </si>
   <si>
-    <t>dmm.measure.func = dmm.FUNC_CAPACITANCE
-dmm.measure.range =
-dmm.measure.read()</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_CONTINUITY
-dmm.measure.read()</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_DIODE
-dmm.measure.read()</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_ACV_FREQUENCY|PERIOD
-dmm.measure.range =
-dmm.measure.displaydigits =
-dmm.measure.read()</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_RESISTANCE|4W_RESISTANCE
-dmm.measure.range =
-dmm.measure.displaydigits =
-dmm.measure.read()</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dmm.measure.func = dmm.FUNC_TEMPERATURE
-dmm.measure.termistor =
-dmm.measure.thermocouple =
-dmm.measure.displaydigits = </t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_TEMPERATURE
-dmm.measure.thermistor =
-dmm.measure.thermocouple =
-dmm.measure.displaydigits =
-dmm.measure.read()</t>
-  </si>
-  <si>
     <t>Resolution ignored for AC and set to 6.5 digits</t>
   </si>
   <si>
-    <t>dmm.measure.func = dmm.FUNC_DC|AC_VOLTAGE
-dmm.measure.range = 
-dmm.measure.displaydigits =
-dmm.measure.read()</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_DCV_AUTO
-dmm.measure.range =
-dmm.measure.displaydigits = 
-dmm.measure.read()</t>
-  </si>
-  <si>
-    <t>dmm.measure.func =</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dmm.measure.range = </t>
-  </si>
-  <si>
-    <t>dmm.measure.range = 
-dmm.measure.displaydigits =</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.func)</t>
-  </si>
-  <si>
     <t>Options are slightly different</t>
   </si>
   <si>
-    <t>dmm.measure.detectorbandwidth =</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.detectorbandwidth)</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.rel.enable)</t>
-  </si>
-  <si>
-    <t>dmm.measure.rel.enable =</t>
-  </si>
-  <si>
-    <t>dmm.measure.rel.level =</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.rel.level)</t>
-  </si>
-  <si>
-    <t>6500 more limited range</t>
-  </si>
-  <si>
-    <t>print(relAutoState)</t>
-  </si>
-  <si>
     <t>Will need to have an auto state, should this also turn rel on?</t>
   </si>
   <si>
-    <t>if dmm.measure.rel.enable do
-    dmm.measure.rel.acquire()
-end</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.range)</t>
-  </si>
-  <si>
-    <t>dmm.measure.autorange =</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.autorange)</t>
-  </si>
-  <si>
-    <t>dmm.measure.nplc =</t>
-  </si>
-  <si>
     <t>34461 Does not have this option</t>
   </si>
   <si>
-    <t>print(dmm.measure.nplc)</t>
-  </si>
-  <si>
-    <t>Should we change displayed digits as well?
-Parameter range is more limited on 6500</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.displaydigits)</t>
-  </si>
-  <si>
-    <t>dmm.measure.autozero.enable|dmm.measure.autozero.once()</t>
-  </si>
-  <si>
-    <t>print(dmm.measure.autozero.enable)</t>
-  </si>
-  <si>
-    <t>dmm.measure.func = dmm.FUNC_DC|AC_CURRENT
-dmm.measure.range =
-dmm.measure.displaydigits =
-dmm.measure.read()</t>
-  </si>
-  <si>
     <t>Display digits ignored fixed at 4.5 dig</t>
   </si>
   <si>
@@ -1643,6 +1471,27 @@
   </si>
   <si>
     <t>Abbreviations</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>6500 more limited range, -1000 to 1000</t>
+  </si>
+  <si>
+    <t>Not currently supported</t>
+  </si>
+  <si>
+    <t>No true secondary function on 6500</t>
+  </si>
+  <si>
+    <t>Not available on 6500</t>
+  </si>
+  <si>
+    <t>NPLC is more limited on 6500</t>
+  </si>
+  <si>
+    <t>Once only works if current function matches</t>
   </si>
 </sst>
 </file>
@@ -1876,26 +1725,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1912,9 +1751,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1924,22 +1760,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1951,26 +1772,14 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2009,7 +1818,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -2049,21 +1858,41 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2081,46 +1910,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2424,1066 +2213,953 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F525"/>
+  <dimension ref="A1:E525"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A484" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D534" sqref="D533:D534"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="94" customWidth="1"/>
-    <col min="5" max="5" width="91.140625" customWidth="1"/>
-    <col min="6" max="6" width="54" customWidth="1"/>
+    <col min="5" max="5" width="54" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="38" t="s">
-        <v>522</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>523</v>
-      </c>
-      <c r="C1" s="40"/>
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
+        <v>479</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>480</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>481</v>
+      </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="39" t="s">
+        <v>478</v>
+      </c>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="36"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="C3" s="28" t="b">
+        <v>1</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B4" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C4" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C5" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B7" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C7" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C8" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B9" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C9" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B10" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C10" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B11" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C11" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B12" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C12" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="46" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D13" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="36"/>
+    </row>
+    <row r="14" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="B14" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C14" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C15" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C16" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E16" s="6"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B17" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C17" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B18" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C18" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E18" s="6"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B19" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C19" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="6"/>
+    </row>
+    <row r="20" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B20" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C20" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="6"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B21" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C21" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B22" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C22" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="36"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="B24" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C24" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E24" s="18"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B25" s="33" t="b">
+        <v>0</v>
+      </c>
+      <c r="C25" s="34" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="19"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D26" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="38"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="B27" s="27" t="b">
+        <v>0</v>
+      </c>
+      <c r="C27" s="28" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B28" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C28" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="22"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B29" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C29" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" s="22"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B30" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C30" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E30" s="22" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B31" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C31" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="22"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B32" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C32" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="22"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B33" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C33" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D33" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E33" s="22"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B34" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C34" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E34" s="22" t="s">
         <v>482</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>478</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="41" t="s">
-        <v>521</v>
-      </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="E2" s="8"/>
-      <c r="F2" s="9"/>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="B3" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="C3" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>470</v>
-      </c>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B4" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C4" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>471</v>
-      </c>
-      <c r="F4" s="24" t="s">
-        <v>520</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B5" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C5" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" s="16" t="s">
-        <v>472</v>
-      </c>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B6" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>473</v>
-      </c>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B7" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C7" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>474</v>
-      </c>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B8" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C8" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="21" t="s">
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B35" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C35" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="22"/>
+    </row>
+    <row r="36" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B36" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C36" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="23" t="s">
         <v>475</v>
       </c>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B9" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C9" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D9" s="27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="28" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B37" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C37" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="22"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B38" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C38" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="22"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B39" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C39" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="22"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B40" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C40" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="22"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B41" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C41" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D41" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="22"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B42" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C42" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B43" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C43" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="E43" s="22" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B44" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="E44" s="22" t="s">
         <v>476</v>
       </c>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B10" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C10" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" s="21" t="s">
-        <v>489</v>
-      </c>
-      <c r="F10" s="5" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B11" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C11" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>480</v>
-      </c>
-      <c r="F11" s="11" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="B12" s="53" t="b">
-        <v>0</v>
-      </c>
-      <c r="C12" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="23" t="s">
-        <v>481</v>
-      </c>
-      <c r="F12" s="6"/>
-    </row>
-    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D13" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="8"/>
-      <c r="F13" s="9"/>
-    </row>
-    <row r="14" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="B14" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="C14" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="15" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B45" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B46" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C46" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B47" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C47" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B48" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C48" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B49" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C49" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E49" s="22" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B50" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C50" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E50" s="23" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B51" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C51" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="E51" s="23" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B52" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C52" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="E52" s="22" t="s">
         <v>484</v>
       </c>
-      <c r="F14" s="13" t="s">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B53" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C53" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B54" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C54" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E54" s="22" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B15" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C15" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>485</v>
-      </c>
-      <c r="F15" s="10"/>
-    </row>
-    <row r="16" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B16" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C16" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>519</v>
-      </c>
-      <c r="F16" s="10"/>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B17" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C17" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>486</v>
-      </c>
-      <c r="F17" s="10"/>
-    </row>
-    <row r="18" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B18" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C18" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="17" t="s">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B55" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C55" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D55" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B56" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C56" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="29" t="b">
+        <v>0</v>
+      </c>
+      <c r="B57" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="C57" s="31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D57" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="29" t="b">
+        <v>1</v>
+      </c>
+      <c r="B58" s="30" t="b">
+        <v>1</v>
+      </c>
+      <c r="C58" s="31" t="b">
+        <v>1</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="E58" s="22" t="s">
         <v>487</v>
       </c>
-      <c r="F18" s="10"/>
-    </row>
-    <row r="19" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B19" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C19" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="26" t="s">
-        <v>488</v>
-      </c>
-      <c r="F19" s="10"/>
-    </row>
-    <row r="20" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B20" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C20" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="17" t="s">
-        <v>490</v>
-      </c>
-      <c r="F20" s="10"/>
-    </row>
-    <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B21" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C21" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>492</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="B22" s="53" t="b">
-        <v>0</v>
-      </c>
-      <c r="C22" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D22" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>493</v>
-      </c>
-      <c r="F22" s="12"/>
-    </row>
-    <row r="23" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D23" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="9"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="B24" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="C24" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="D24" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E24" s="31" t="s">
-        <v>494</v>
-      </c>
-      <c r="F24" s="29"/>
-    </row>
-    <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="B25" s="53" t="b">
-        <v>0</v>
-      </c>
-      <c r="C25" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="32" t="s">
-        <v>23</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>497</v>
-      </c>
-      <c r="F25" s="30"/>
-    </row>
-    <row r="26" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="E26" s="34"/>
-      <c r="F26" s="35"/>
-    </row>
-    <row r="27" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="46" t="b">
-        <v>1</v>
-      </c>
-      <c r="B27" s="47" t="b">
-        <v>0</v>
-      </c>
-      <c r="C27" s="48" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="17" t="s">
-        <v>496</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>491</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B28" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C28" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="21" t="s">
-        <v>496</v>
-      </c>
-      <c r="F28" s="36"/>
-    </row>
-    <row r="29" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B29" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C29" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>470</v>
-      </c>
-      <c r="F29" s="36"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B30" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C30" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>499</v>
-      </c>
-      <c r="F30" s="36" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B31" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C31" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E31" s="16" t="s">
-        <v>500</v>
-      </c>
-      <c r="F31" s="36"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B32" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C32" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>502</v>
-      </c>
-      <c r="F32" s="36"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B33" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C33" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E33" s="16" t="s">
-        <v>501</v>
-      </c>
-      <c r="F33" s="36"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B34" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C34" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="E34" s="25" t="s">
-        <v>503</v>
-      </c>
-      <c r="F34" s="36" t="s">
-        <v>505</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B35" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C35" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>504</v>
-      </c>
-      <c r="F35" s="36"/>
-    </row>
-    <row r="36" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B36" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C36" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="21" t="s">
-        <v>508</v>
-      </c>
-      <c r="F36" s="37" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B37" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C37" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E37" s="17" t="s">
-        <v>506</v>
-      </c>
-      <c r="F37" s="36"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B38" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C38" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="E38" s="21" t="s">
-        <v>495</v>
-      </c>
-      <c r="F38" s="36"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B39" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C39" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="16" t="s">
-        <v>509</v>
-      </c>
-      <c r="F39" s="36"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B40" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C40" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="E40" s="20" t="s">
-        <v>510</v>
-      </c>
-      <c r="F40" s="36"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B41" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C41" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="E41" s="16" t="s">
-        <v>511</v>
-      </c>
-      <c r="F41" s="36"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B42" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C42" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>36</v>
-      </c>
-      <c r="E42" s="25"/>
-      <c r="F42" s="36"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B43" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C43" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D43" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="36"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="B44" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C44" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D44" s="44" t="s">
-        <v>38</v>
-      </c>
-      <c r="E44" s="44"/>
-      <c r="F44" s="36" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="B45" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C45" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D45" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="45"/>
-      <c r="F45" s="36" t="s">
-        <v>513</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="B46" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C46" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D46" s="44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E46" s="44"/>
-      <c r="F46" s="36"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="B47" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C47" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D47" s="45" t="s">
-        <v>41</v>
-      </c>
-      <c r="E47" s="45"/>
-      <c r="F47" s="36"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="B48" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C48" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="44" t="s">
-        <v>42</v>
-      </c>
-      <c r="E48" s="44"/>
-      <c r="F48" s="36"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" s="49" t="b">
-        <v>0</v>
-      </c>
-      <c r="B49" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C49" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D49" s="45" t="s">
-        <v>43</v>
-      </c>
-      <c r="E49" s="45"/>
-      <c r="F49" s="36"/>
-    </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B50" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C50" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D50" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>512</v>
-      </c>
-      <c r="F50" s="37" t="s">
-        <v>515</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B51" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C51" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D51" s="27" t="s">
-        <v>45</v>
-      </c>
-      <c r="E51" s="27" t="s">
-        <v>514</v>
-      </c>
-      <c r="F51" s="36"/>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B52" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C52" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D52" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="E52" s="25"/>
-      <c r="F52" s="36"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B53" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C53" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D53" s="27" t="s">
-        <v>47</v>
-      </c>
-      <c r="E53" s="27"/>
-      <c r="F53" s="36"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B54" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C54" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D54" s="20" t="s">
-        <v>48</v>
-      </c>
-      <c r="E54" s="20" t="s">
-        <v>479</v>
-      </c>
-      <c r="F54" s="36"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B55" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C55" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D55" s="16" t="s">
-        <v>49</v>
-      </c>
-      <c r="E55" s="16" t="s">
-        <v>516</v>
-      </c>
-      <c r="F55" s="36"/>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B56" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C56" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D56" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="E56" s="25"/>
-      <c r="F56" s="36"/>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A57" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B57" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C57" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>51</v>
-      </c>
-      <c r="E57" s="27"/>
-      <c r="F57" s="36"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="49" t="b">
-        <v>1</v>
-      </c>
-      <c r="B58" s="50" t="b">
-        <v>0</v>
-      </c>
-      <c r="C58" s="51" t="b">
-        <v>0</v>
-      </c>
-      <c r="D58" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E58" s="20" t="s">
-        <v>517</v>
-      </c>
-      <c r="F58" s="36"/>
-    </row>
-    <row r="59" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="52" t="b">
-        <v>1</v>
-      </c>
-      <c r="B59" s="53" t="b">
-        <v>0</v>
-      </c>
-      <c r="C59" s="54" t="b">
-        <v>0</v>
-      </c>
-      <c r="D59" s="18" t="s">
+    </row>
+    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="32" t="b">
+        <v>1</v>
+      </c>
+      <c r="B59" s="33" t="b">
+        <v>1</v>
+      </c>
+      <c r="C59" s="34" t="b">
+        <v>1</v>
+      </c>
+      <c r="D59" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="E59" s="18" t="s">
-        <v>518</v>
-      </c>
-      <c r="F59" s="30"/>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E59" s="19"/>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D60" s="1" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D61" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D62" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D63" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="47"/>
+      <c r="B64" s="48"/>
       <c r="D64" t="s">
         <v>60</v>
       </c>
@@ -5795,33 +5471,17 @@
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D23:F23"/>
-    <mergeCell ref="D26:F26"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D26:E26"/>
     <mergeCell ref="A2:C2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A3:A12 A24:A25 A27:A59 A14:A22">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+  <conditionalFormatting sqref="A3:C12 A14:C22 A24:C25 A27:C59">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B3:B12 B24:B25 B27:B59 B14:B22">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
-      <formula>FALSE</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C3:C12 C24:C25 C27:C59 C14:C22">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>